<commit_message>
Hospital, districts and weather dataset preprocessed
</commit_message>
<xml_diff>
--- a/Code/Prep codes/test_dir/result.xlsx
+++ b/Code/Prep codes/test_dir/result.xlsx
@@ -718,2758 +718,2758 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20220625_dengue_all</t>
+          <t>20220624_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20220626_dengue_all</t>
+          <t>20220625_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>20220627_dengue_all</t>
+          <t>20220626_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>20220629_dengue_all</t>
+          <t>20220627_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>20220701_dengue_all</t>
+          <t>20220629_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20220702_dengue_all</t>
+          <t>20220701_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20220703_dengue_all</t>
+          <t>20220702_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20220704_dengue_all</t>
+          <t>20220703_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>20220705_dengue_all</t>
+          <t>20220704_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>20220706_dengue_all</t>
+          <t>20220705_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>20220707_dengue_all</t>
+          <t>20220706_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>20220708_dengue_all</t>
+          <t>20220707_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>20220709_dengue_all</t>
+          <t>20220708_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>20220710_dengue_all</t>
+          <t>20220709_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20220711_dengue_all</t>
+          <t>20220710_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>20220712_dengue_all</t>
+          <t>20220711_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>20220713_dengue_all</t>
+          <t>20220712_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>20220714_dengue_all</t>
+          <t>20220713_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>20220715_dengue_all</t>
+          <t>20220714_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>20220716_dengue_all</t>
+          <t>20220715_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>20220717_dengue_all</t>
+          <t>20220716_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>20220718_dengue_all</t>
+          <t>20220717_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>20220719_dengue_all</t>
+          <t>20220718_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>20220720_dengue_all</t>
+          <t>20220719_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>20220721_dengue_all</t>
+          <t>20220720_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>20220722_dengue_all</t>
+          <t>20220721_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>20220723_dengue_all</t>
+          <t>20220722_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>20220724_dengue_all</t>
+          <t>20220723_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>20220726_dengue_all</t>
+          <t>20220724_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>20220728_dengue_all</t>
+          <t>20220726_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>20220729_dengue_all</t>
+          <t>20220728_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>20220730_dengue_all</t>
+          <t>20220729_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>20220731_dengue_all</t>
+          <t>20220730_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>20220801_dengue_all</t>
+          <t>20220731_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>20220802_dengue_all</t>
+          <t>20220801_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>20220803_dengue_all</t>
+          <t>20220802_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>20220804_dengue_all</t>
+          <t>20220803_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>20220805_dengue_all</t>
+          <t>20220804_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>20220806_dengue_all</t>
+          <t>20220805_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>20220807_dengue_all</t>
+          <t>20220806_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>20220808_dengue_all</t>
+          <t>20220807_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>20220810_dengue_all</t>
+          <t>20220808_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>20220811_dengue_all</t>
+          <t>20220810_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>20220812_dengue_all</t>
+          <t>20220811_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>20220813_dengue_all</t>
+          <t>20220812_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>20220814_dengue_all</t>
+          <t>20220813_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>20220815_dengue_all</t>
+          <t>20220814_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>20220817_dengue_all</t>
+          <t>20220815_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>20220818_dengue_all</t>
+          <t>20220817_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>20220819_dengue_all</t>
+          <t>20220818_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>20220820_dengue_all</t>
+          <t>20220819_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>20220821_dengue_all</t>
+          <t>20220820_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>20220822_dengue_all</t>
+          <t>20220821_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>20220823_dengue_all</t>
+          <t>20220822_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>20220824_dengue_all</t>
+          <t>20220823_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>20220825_dengue_all</t>
+          <t>20220824_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>20220826_dengue_all</t>
+          <t>20220825_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>20220827_dengue_all</t>
+          <t>20220826_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>20220828_dengue_all</t>
+          <t>20220827_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>20220829_dengue_all</t>
+          <t>20220828_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>20220830_dengue_all</t>
+          <t>20220829_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>20220901_dengue_all</t>
+          <t>20220830_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>20220902_dengue_all</t>
+          <t>20220901_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>20220903_dengue_all</t>
+          <t>20220902_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>20220904_dengue_all</t>
+          <t>20220903_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>20220905_dengue_all</t>
+          <t>20220904_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>20220906_dengue_all</t>
+          <t>20220905_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>20220907_dengue_all</t>
+          <t>20220906_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>20220908_dengue_all</t>
+          <t>20220907_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>20220910_dengue_all</t>
+          <t>20220908_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>20220911_dengue_all</t>
+          <t>20220910_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>20220912_dengue_all</t>
+          <t>20220911_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>20220913_dengue_all</t>
+          <t>20220912_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>20220914_dengue_all</t>
+          <t>20220913_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>20220915_dengue_all</t>
+          <t>20220914_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>20220916_dengue_all</t>
+          <t>20220915_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>20220917_dengue_all</t>
+          <t>20220916_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>20220918_dengue_all</t>
+          <t>20220917_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>20220919_dengue_all</t>
+          <t>20220918_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>20220920_dengue_all</t>
+          <t>20220919_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>20220921_dengue_all</t>
+          <t>20220920_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>20220922_dengue_all</t>
+          <t>20220921_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>20220923_dengue_all</t>
+          <t>20220922_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>20220924_dengue_all</t>
+          <t>20220923_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>20220925_dengue_all</t>
+          <t>20220924_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>20220926_dengue_all</t>
+          <t>20220925_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>20220927_dengue_all</t>
+          <t>20220926_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>20220928_dengue_all</t>
+          <t>20220927_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>20220929_dengue_all</t>
+          <t>20220928_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>20221001_dengue_all</t>
+          <t>20220929_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>20221002_dengue_all</t>
+          <t>20221001_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>20221003_dengue_all</t>
+          <t>20221002_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>20221004_dengue_all</t>
+          <t>20221003_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>20221005_dengue_all</t>
+          <t>20221004_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>20221006_dengue_all</t>
+          <t>20221005_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>20221007_dengue_all</t>
+          <t>20221006_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>20221008_dengue_all</t>
+          <t>20221007_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>20221011_dengue_all</t>
+          <t>20221008_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>20221012_dengue_all</t>
+          <t>20221011_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>20221013_dengue_all</t>
+          <t>20221012_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>20221014_dengue_all</t>
+          <t>20221013_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>20221015_dengue_all</t>
+          <t>20221014_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>20221016_dengue_all</t>
+          <t>20221015_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>20221017_dengue_all</t>
+          <t>20221016_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>20221018_dengue_all</t>
+          <t>20221017_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>20221019_dengue_all</t>
+          <t>20221018_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>20221020_dengue_all</t>
+          <t>20221019_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>20221021_dengue_all</t>
+          <t>20221020_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>20221022_dengue_all</t>
+          <t>20221021_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>20221023_dengue_all</t>
+          <t>20221022_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>20221024_dengue_all</t>
+          <t>20221023_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>20221025_dengue_all</t>
+          <t>20221024_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>20221026_dengue_all</t>
+          <t>20221025_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>20221027_dengue_all</t>
+          <t>20221026_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>20221028_dengue_all</t>
+          <t>20221027_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>20221031_dengue_all</t>
+          <t>20221028_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>20221030_dengue_all</t>
+          <t>20221031_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>20221101_dengue_all</t>
+          <t>20221030_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>20221102_dengue_all</t>
+          <t>20221101_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>20221103_dengue_all</t>
+          <t>20221102_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>20221104_dengue_all</t>
+          <t>20221103_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>20221105_dengue_all</t>
+          <t>20221104_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>20221107_dengue_all</t>
+          <t>20221105_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>20221108_dengue_all</t>
+          <t>20221107_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>20221109_dengue_all</t>
+          <t>20221108_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>20221110_dengue_all</t>
+          <t>20221109_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>20221111_dengue_all</t>
+          <t>20221110_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>20221112_dengue_all</t>
+          <t>20221111_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>20221113_dengue_all</t>
+          <t>20221112_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>20221114_dengue_all</t>
+          <t>20221113_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>20221115_dengue_all</t>
+          <t>20221114_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>20221116_dengue_all</t>
+          <t>20221115_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>20221117_dengue_all</t>
+          <t>20221116_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>20221118_dengue_all</t>
+          <t>20221117_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>20221119_dengue_all</t>
+          <t>20221118_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>20221120_dengue_all</t>
+          <t>20221119_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>20221121_dengue_all</t>
+          <t>20221120_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>20221122_dengue_all</t>
+          <t>20221121_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>20221123_dengue_all</t>
+          <t>20221122_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>20221124_dengue_all</t>
+          <t>20221123_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>20221125_dengue_all</t>
+          <t>20221124_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>20221126_dengue_all</t>
+          <t>20221125_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>20221127_dengue_all</t>
+          <t>20221126_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>20221201_dengue_all</t>
+          <t>20221127_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>20221202_dengue_all</t>
+          <t>20221201_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>20221203_dengue_all</t>
+          <t>20221202_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>20221204_dengue_all</t>
+          <t>20221203_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>20221205_dengue_all</t>
+          <t>20221204_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>20221206_dengue_all</t>
+          <t>20221205_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>20221207_dengue_all</t>
+          <t>20221206_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>20221208_dengue_all</t>
+          <t>20221207_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>20221209_dengue_all</t>
+          <t>20221208_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>20221210_dengue_all</t>
+          <t>20221209_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>20221211_dengue_all</t>
+          <t>20221210_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>20221212_dengue_all</t>
+          <t>20221211_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>20221213_dengue_all</t>
+          <t>20221212_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>20221214_dengue_all</t>
+          <t>20221213_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>20221215_dengue_all</t>
+          <t>20221214_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>20221216_dengue_all</t>
+          <t>20221215_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>20221217_dengue_all</t>
+          <t>20221216_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>20221218_dengue_all</t>
+          <t>20221217_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>20221219_dengue_all</t>
+          <t>20221218_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>20221220_dengue_all</t>
+          <t>20221219_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>20221221_dengue_all</t>
+          <t>20221220_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>20221222_dengue_all</t>
+          <t>20221221_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>20221223_dengue_all</t>
+          <t>20221222_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>20221224_dengue_all</t>
+          <t>20221223_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>20221225_dengue_all</t>
+          <t>20221224_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>20221226_dengue_all</t>
+          <t>20221225_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>20221227_dengue_all</t>
+          <t>20221226_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>20221228_dengue_all</t>
+          <t>20221227_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>20221229_dengue_all</t>
+          <t>20221228_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>20221230_dengue_all</t>
+          <t>20221229_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>20230101_dengue_all</t>
+          <t>20221230_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>20230102_dengue_all</t>
+          <t>20230101_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>20230103_dengue_all</t>
+          <t>20230102_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>20230104_dengue_all</t>
+          <t>20230103_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>20230105_dengue_all</t>
+          <t>20230104_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>20230106_dengue_all</t>
+          <t>20230105_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>20230107_dengue_all</t>
+          <t>20230106_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>20230108_dengue_all</t>
+          <t>20230107_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>20230109_dengue_all</t>
+          <t>20230108_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>20230110_dengue_all</t>
+          <t>20230109_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>20230111_dengue_all</t>
+          <t>20230110_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>20230112_dengue_all</t>
+          <t>20230111_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>20230113_dengue_all</t>
+          <t>20230112_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>20230114_dengue_all</t>
+          <t>20230113_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>20230115_dengue_all</t>
+          <t>20230114_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>20230116_dengue_all</t>
+          <t>20230115_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>20230117_dengue_all</t>
+          <t>20230116_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>20230118_dengue_all</t>
+          <t>20230117_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>20230119_dengue_all</t>
+          <t>20230118_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>20230120_dengue_all</t>
+          <t>20230119_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>20230121_dengue_all</t>
+          <t>20230120_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>20230122_dengue_all</t>
+          <t>20230121_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>20230123_dengue_all</t>
+          <t>20230122_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>20230124_dengue_all</t>
+          <t>20230123_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>20230125_dengue_all</t>
+          <t>20230124_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>20230126_dengue_all</t>
+          <t>20230125_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>20230127_dengue_all</t>
+          <t>20230126_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>20230128_dengue_all</t>
+          <t>20230127_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>20230129_dengue_all</t>
+          <t>20230128_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>20230130_dengue_all</t>
+          <t>20230129_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>20230131_dengue_all</t>
+          <t>20230130_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>20230201_dengue_all</t>
+          <t>20230131_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>20230202_dengue_all</t>
+          <t>20230201_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>20230203_dengue_all</t>
+          <t>20230202_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>20230204_dengue_all</t>
+          <t>20230203_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>20230206_dengue_all</t>
+          <t>20230204_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>20230207_dengue_all</t>
+          <t>20230206_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>20230208_dengue_all</t>
+          <t>20230207_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>20230209_dengue_all</t>
+          <t>20230208_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>20230210_dengue_all</t>
+          <t>20230209_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>20230211_dengue_all</t>
+          <t>20230210_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>20230212_dengue_all</t>
+          <t>20230211_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>20230213_dengue_all</t>
+          <t>20230212_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>20230214_dengue_all</t>
+          <t>20230213_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>20230215_dengue_all</t>
+          <t>20230214_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>20230217_dengue_all</t>
+          <t>20230215_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>20230218_dengue_all</t>
+          <t>20230217_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>20230219_dengue_all</t>
+          <t>20230218_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>20230220_dengue_all</t>
+          <t>20230219_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>20230221_dengue_all</t>
+          <t>20230220_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>20230222_dengue_all</t>
+          <t>20230221_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>20230223_dengue_all</t>
+          <t>20230222_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>20230224_dengue_all</t>
+          <t>20230223_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>20230225_dengue_all</t>
+          <t>20230224_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>20230226_dengue_all</t>
+          <t>20230225_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>20230227_dengue_all</t>
+          <t>20230226_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>20230228_dengue_all</t>
+          <t>20230227_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>20230301_dengue_all</t>
+          <t>20230228_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>20230302_dengue_all</t>
+          <t>20230301_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>20230303_dengue_all</t>
+          <t>20230302_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>20230304_dengue_all</t>
+          <t>20230303_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>20230305_dengue_all</t>
+          <t>20230304_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>20230306_dengue_all</t>
+          <t>20230305_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>20230307_dengue_all</t>
+          <t>20230306_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>20230308_dengue_all</t>
+          <t>20230307_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>20230309_dengue_all</t>
+          <t>20230308_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>20230310_dengue_all</t>
+          <t>20230309_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>20230311_dengue_all</t>
+          <t>20230310_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>20230312_dengue_all</t>
+          <t>20230311_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>20230313_dengue_all</t>
+          <t>20230312_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>20230314_dengue_all</t>
+          <t>20230313_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>20230315_dengue_all</t>
+          <t>20230314_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>20230316_dengue_all</t>
+          <t>20230315_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>20230317_dengue_all</t>
+          <t>20230316_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>20230318_dengue_all</t>
+          <t>20230317_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>20230319_dengue_all</t>
+          <t>20230318_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>20230320_dengue_all</t>
+          <t>20230319_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>20230321_dengue_all</t>
+          <t>20230320_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>20230322_dengue_all</t>
+          <t>20230321_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>20230323_dengue_all</t>
+          <t>20230322_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>20230324_dengue_all</t>
+          <t>20230323_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>20230325_dengue_all</t>
+          <t>20230324_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>20230326_dengue_all</t>
+          <t>20230325_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>20230327_dengue_all</t>
+          <t>20230326_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>20230328_dengue_all</t>
+          <t>20230327_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>20230329_dengue_all</t>
+          <t>20230328_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>20230330_dengue_all</t>
+          <t>20230329_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>20230331_dengue_all</t>
+          <t>20230330_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>20230401_dengue_all</t>
+          <t>20230331_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>20230402_dengue_all</t>
+          <t>20230401_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>20230403_dengue_all</t>
+          <t>20230402_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>20230404_dengue_all</t>
+          <t>20230403_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>20230405_dengue_all</t>
+          <t>20230404_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>20230406_dengue_all</t>
+          <t>20230405_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>20230407_dengue_all</t>
+          <t>20230406_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>20230408_dengue_all</t>
+          <t>20230407_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>20230409_dengue_all</t>
+          <t>20230408_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>20230410_dengue_all</t>
+          <t>20230409_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>20230411_dengue_all</t>
+          <t>20230410_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>20230412_dengue_all</t>
+          <t>20230411_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>20230413_dengue_all</t>
+          <t>20230412_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>20230414_dengue_all</t>
+          <t>20230413_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>20230415_dengue_all</t>
+          <t>20230414_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>20230416_dengue_all</t>
+          <t>20230415_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>20230417_dengue_all</t>
+          <t>20230416_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>20230418_dengue_all</t>
+          <t>20230417_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>20230419_dengue_all</t>
+          <t>20230418_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>20230420_dengue_all</t>
+          <t>20230419_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>20230421_dengue_all</t>
+          <t>20230420_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>20230422_dengue_all</t>
+          <t>20230421_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>20230423_dengue_all</t>
+          <t>20230422_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>20230424_dengue_all</t>
+          <t>20230423_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>20230425_dengue_all</t>
+          <t>20230424_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>20230426_dengue_all</t>
+          <t>20230425_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>20230427_dengue_all</t>
+          <t>20230426_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>20230428_dengue_all</t>
+          <t>20230427_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>20230429_dengue_all</t>
+          <t>20230428_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>20230430_dengue_all</t>
+          <t>20230429_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>20230501_dengue_all</t>
+          <t>20230430_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>20230502_dengue_all</t>
+          <t>20230501_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>20230503_dengue_all</t>
+          <t>20230502_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>20230504_dengue_all</t>
+          <t>20230503_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>20230505_dengue_all</t>
+          <t>20230504_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>20230506_dengue_all</t>
+          <t>20230505_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>20230507_dengue_all</t>
+          <t>20230506_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>20230508_dengue_all</t>
+          <t>20230507_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>20230509_dengue_all</t>
+          <t>20230508_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>20230510_dengue_all</t>
+          <t>20230509_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>20230511_dengue_all</t>
+          <t>20230510_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>20230512_dengue_all</t>
+          <t>20230511_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>20230514_dengue_all</t>
+          <t>20230512_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>20230515_dengue_all</t>
+          <t>20230514_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>20230516_dengue_all</t>
+          <t>20230515_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>20230517_dengue_all</t>
+          <t>20230516_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>20230518_dengue_all</t>
+          <t>20230517_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>20230519_dengue_all</t>
+          <t>20230518_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>20230520_dengue_all</t>
+          <t>20230519_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>20230521_dengue_all</t>
+          <t>20230520_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>20230522_dengue_all</t>
+          <t>20230521_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>20230523_dengue_all</t>
+          <t>20230522_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>20230524_dengue_all</t>
+          <t>20230523_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>20230525_dengue_all</t>
+          <t>20230524_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>20230526_dengue_all</t>
+          <t>20230525_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>20230527_dengue_all</t>
+          <t>20230526_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>20230528_dengue_all</t>
+          <t>20230527_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>20230529_dengue_all</t>
+          <t>20230528_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>20230530_dengue_all</t>
+          <t>20230529_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>20230531_dengue_all</t>
+          <t>20230530_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>20230601_dengue_all</t>
+          <t>20230531_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>20230602_dengue_all</t>
+          <t>20230601_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>20230603_dengue_all</t>
+          <t>20230602_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>20230604_dengue_all</t>
+          <t>20230603_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>20230605_dengue_all</t>
+          <t>20230604_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>20230606_dengue_all</t>
+          <t>20230605_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>20230607_dengue_all</t>
+          <t>20230606_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>20230608_dengue_all</t>
+          <t>20230607_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>20230609_dengue_all</t>
+          <t>20230608_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>20230610_dengue_all</t>
+          <t>20230609_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>20230611_dengue_all</t>
+          <t>20230610_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>20230612_dengue_all</t>
+          <t>20230611_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>20230613_dengue_all</t>
+          <t>20230612_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>20230614_dengue_all</t>
+          <t>20230613_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>20230615_dengue_all</t>
+          <t>20230614_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>20230616_dengue_all</t>
+          <t>20230615_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>20230617_dengue_all</t>
+          <t>20230616_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>20230618_dengue_all</t>
+          <t>20230617_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>20230619_dengue_all</t>
+          <t>20230618_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>20230620_dengue_all</t>
+          <t>20230619_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>20230621_dengue_all</t>
+          <t>20230620_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>20230622_dengue_all</t>
+          <t>20230621_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>20230623_dengue_all</t>
+          <t>20230622_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>20230624_dengue_all</t>
+          <t>20230623_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>20230625_dengue_all</t>
+          <t>20230624_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>20230626_dengue_all</t>
+          <t>20230625_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>20230627_dengue_all</t>
+          <t>20230626_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>20230628_dengue_all</t>
+          <t>20230627_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>20230629_dengue_all</t>
+          <t>20230628_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>20230630_dengue_all</t>
+          <t>20230629_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>20230701_dengue_all</t>
+          <t>20230630_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>20230702_dengue_all</t>
+          <t>20230701_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>20230703_dengue_all</t>
+          <t>20230702_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>20230704_dengue_all</t>
+          <t>20230703_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>20230705_dengue_all</t>
+          <t>20230704_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>20230706_dengue_all</t>
+          <t>20230705_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>20230707_dengue_all</t>
+          <t>20230706_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>20230708_dengue_all</t>
+          <t>20230707_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>20230709_dengue_all</t>
+          <t>20230708_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>20230710_dengue_all</t>
+          <t>20230709_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>20230711_dengue_all</t>
+          <t>20230710_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>20230712_dengue_all</t>
+          <t>20230711_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>20230713_dengue_all</t>
+          <t>20230712_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>20230714_dengue_all</t>
+          <t>20230713_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>20230715_dengue_all</t>
+          <t>20230714_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>20230716_dengue_all</t>
+          <t>20230715_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>20230717_dengue_all</t>
+          <t>20230716_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>20230718_dengue_all</t>
+          <t>20230717_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>20230719_dengue_all</t>
+          <t>20230718_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>20230720_dengue_all</t>
+          <t>20230719_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>20230721_dengue_all</t>
+          <t>20230720_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>20230722_dengue_all</t>
+          <t>20230721_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>20230723_dengue_all</t>
+          <t>20230722_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>20230725_dengue_all</t>
+          <t>20230723_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>20230726_dengue_all</t>
+          <t>20230725_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>20230727_dengue_all</t>
+          <t>20230726_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>20230728_dengue_all</t>
+          <t>20230727_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>20230729_dengue_all</t>
+          <t>20230728_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>Dengue_20190901</t>
+          <t>20230729_dengue_all</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>Dengue_20190902</t>
+          <t>Dengue_20190901</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>Dengue_20190903</t>
+          <t>Dengue_20190902</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>Dengue_20190906</t>
+          <t>Dengue_20190903</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>Dengue_20190907</t>
+          <t>Dengue_20190906</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>Dengue_20190908</t>
+          <t>Dengue_20190907</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>Dengue_20190910</t>
+          <t>Dengue_20190908</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>Dengue_20190911</t>
+          <t>Dengue_20190910</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>Dengue_20190912</t>
+          <t>Dengue_20190911</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>Dengue_20190913</t>
+          <t>Dengue_20190912</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>Dengue_20190914</t>
+          <t>Dengue_20190913</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>Dengue_20190915</t>
+          <t>Dengue_20190914</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>Dengue_20190916</t>
+          <t>Dengue_20190915</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>Dengue_20190917</t>
+          <t>Dengue_20190916</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>Dengue_20190918</t>
+          <t>Dengue_20190917</t>
         </is>
       </c>
     </row>

</xml_diff>